<commit_message>
fix problem with absolute coordinates in ArrayEval
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/array.xlsx
+++ b/test-data/spreadsheet/array.xlsx
@@ -1165,8 +1165,8 @@
         <v>17</v>
       </c>
       <c r="F18">
-        <f t="array" ref="F18">PRODUCT(D2:D17/E2:E17)</f>
-        <v>2.2277128597140037E-42</v>
+        <f t="array" ref="F18">SUM(D2:D17+F2:F17)</f>
+        <v>189691</v>
       </c>
       <c r="H18">
         <f>1/2</f>

</xml_diff>

<commit_message>
add feature for 3 and more args in array formula; Add tests
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/array.xlsx
+++ b/test-data/spreadsheet/array.xlsx
@@ -1165,8 +1165,8 @@
         <v>17</v>
       </c>
       <c r="F18">
-        <f t="array" ref="F18">SUM(D2:D17+F2:F17)</f>
-        <v>189691</v>
+        <f t="array" ref="F18">SUM(D2:D17+F2:F17+A2:A17)</f>
+        <v>189827</v>
       </c>
       <c r="H18">
         <f>1/2</f>

</xml_diff>